<commit_message>
myapp DAO, observer pattern
</commit_message>
<xml_diff>
--- a/myapp/app/data.xlsx
+++ b/myapp/app/data.xlsx
@@ -6,15 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="users" r:id="rId6" sheetId="8"/>
-    <sheet name="boards" r:id="rId5" sheetId="9"/>
-    <sheet name="projects" r:id="rId7" sheetId="10"/>
+    <sheet name="users" r:id="rId6" sheetId="29"/>
+    <sheet name="boards" r:id="rId5" sheetId="30"/>
+    <sheet name="projects" r:id="rId7" sheetId="31"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="88">
   <si>
     <t>no</t>
   </si>
@@ -230,6 +230,54 @@
   </si>
   <si>
     <t>66</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user7@test.co</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>010-1111-7777</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>2024-07-26 11:21:36</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user8@test.com</t>
+  </si>
+  <si>
+    <t>8888</t>
+  </si>
+  <si>
+    <t>010-1111-8888</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>2024-07-26 16:46:35</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>77</t>
   </si>
 </sst>
 </file>
@@ -272,9 +320,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -285,19 +333,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -305,39 +350,33 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -345,19 +384,84 @@
         <v>20</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>10</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -365,7 +469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -378,16 +482,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -395,33 +499,33 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>10</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -429,16 +533,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -446,16 +550,16 @@
         <v>48</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -463,16 +567,16 @@
         <v>55</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -480,9 +584,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -496,13 +600,16 @@
         <v>25</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="2">
@@ -510,16 +617,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>45</v>
+        <v>33</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -527,16 +637,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>10</v>
+        <v>67</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -544,16 +657,39 @@
         <v>20</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>45</v>
+        <v>71</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>